<commit_message>
Adding generated reports from pipeline run
</commit_message>
<xml_diff>
--- a/reports/security_reports.xlsx
+++ b/reports/security_reports.xlsx
@@ -17863,7 +17863,7 @@
       </c>
       <c r="I217" t="inlineStr">
         <is>
-          <t>http://www.openwall.com/lists/oss-security/2024/11/18/2, https://access.redhat.com/security/cve/CVE-2024-52316, https://github.com/apache/tomcat, https://github.com/apache/tomcat/commit/6d097a66746635df6880fe7662a792156b0eca14, https://github.com/apache/tomcat/commit/7532f9dc4a8c37ec958f79dc82c4924a6c539223, https://github.com/apache/tomcat/commit/7532f9dc4a8c37ec958f79dc82c4924a6c539223 (9.0.96), https://github.com/apache/tomcat/commit/acc2f01395f895980f5d8a64573fcc1bade13369, https://github.com/apache/tomcat/commit/acc2f01395f895980f5d8a64573fcc1bade13369 (10.1.31), https://linux.oracle.com/cve/CVE-2024-52316.html, https://linux.oracle.com/errata/ELSA-2025-7497.html, https://lists.apache.org/thread/lopzlqh91jj9n334g02om08sbysdb928, https://nvd.nist.gov/vuln/detail/CVE-2024-52316, https://security.netapp.com/advisory/ntap-20250124-0003, https://security.netapp.com/advisory/ntap-20250124-0003/, https://www.cve.org/CVERecord?id=CVE-2024-52316</t>
+          <t>http://www.openwall.com/lists/oss-security/2024/11/18/2, https://access.redhat.com/errata/RHSA-2025:7497, https://access.redhat.com/security/cve/CVE-2024-52316, https://bugzilla.redhat.com/2326972, https://bugzilla.redhat.com/2332815, https://bugzilla.redhat.com/2351129, https://errata.almalinux.org/10/ALSA-2025-7497.html, https://github.com/apache/tomcat, https://github.com/apache/tomcat/commit/6d097a66746635df6880fe7662a792156b0eca14, https://github.com/apache/tomcat/commit/7532f9dc4a8c37ec958f79dc82c4924a6c539223, https://github.com/apache/tomcat/commit/7532f9dc4a8c37ec958f79dc82c4924a6c539223 (9.0.96), https://github.com/apache/tomcat/commit/acc2f01395f895980f5d8a64573fcc1bade13369, https://github.com/apache/tomcat/commit/acc2f01395f895980f5d8a64573fcc1bade13369 (10.1.31), https://linux.oracle.com/cve/CVE-2024-52316.html, https://linux.oracle.com/errata/ELSA-2025-7497.html, https://lists.apache.org/thread/lopzlqh91jj9n334g02om08sbysdb928, https://nvd.nist.gov/vuln/detail/CVE-2024-52316, https://security.netapp.com/advisory/ntap-20250124-0003, https://security.netapp.com/advisory/ntap-20250124-0003/, https://www.cve.org/CVERecord?id=CVE-2024-52316</t>
         </is>
       </c>
       <c r="J217" t="inlineStr">
@@ -18229,7 +18229,7 @@
       </c>
       <c r="I223" t="inlineStr">
         <is>
-          <t>http://www.openwall.com/lists/oss-security/2024/12/17/5, http://www.openwall.com/lists/oss-security/2024/12/17/6, http://www.openwall.com/lists/oss-security/2024/12/18/1, https://access.redhat.com/security/cve/CVE-2024-54677, https://github.com/apache/tomcat, https://github.com/apache/tomcat/commit/1d88dd3ffaed76188dd4ee32ce77709ce6e153cd, https://github.com/apache/tomcat/commit/1d88dd3ffaed76188dd4ee32ce77709ce6e153cd (9.0.98), https://github.com/apache/tomcat/commit/3315a9027a7eaab18f42625b97b569940ff1365d, https://github.com/apache/tomcat/commit/3315a9027a7eaab18f42625b97b569940ff1365d (9.0.98), https://github.com/apache/tomcat/commit/4a335c6dcba8d6f8a54629eda392a50da267bdf4, https://github.com/apache/tomcat/commit/4d5cc6538d91386f950373ac8120e98c2c78ed3a, https://github.com/apache/tomcat/commit/4d5cc6538d91386f950373ac8120e98c2c78ed3a (9.0.98), https://github.com/apache/tomcat/commit/4f0236606961176257b883213e1621b1859ed746, https://github.com/apache/tomcat/commit/54e56495e9a106218efe9fc9c79d976c0032bbfd, https://github.com/apache/tomcat/commit/54e56495e9a106218efe9fc9c79d976c0032bbfd (10.1.34), https://github.com/apache/tomcat/commit/721544ea28e92549824b106be954a9f411867a1c, https://github.com/apache/tomcat/commit/721544ea28e92549824b106be954a9f411867a1c (9.0.98), https://github.com/apache/tomcat/commit/722814668708c42a61b0c1e340b15bc2b785c0d1, https://github.com/apache/tomcat/commit/75ff7e8622edcc024b268677aa789ee8f0880ecc, https://github.com/apache/tomcat/commit/75ff7e8622edcc024b268677aa789ee8f0880ecc (9.0.98), https://github.com/apache/tomcat/commit/84065e26ca4555e63a922bb29b13b0a1c86b7654, https://github.com/apache/tomcat/commit/84065e26ca4555e63a922bb29b13b0a1c86b7654 (9.0.98), https://github.com/apache/tomcat/commit/84c4af76e7a10fc7f8630ce62e6a46632ea4a90e, https://github.com/apache/tomcat/commit/84c4af76e7a10fc7f8630ce62e6a46632ea4a90e (9.0.98), https://github.com/apache/tomcat/commit/9ffd23fc27f5d1fc95bf97e5cea175c8968f4533, https://github.com/apache/tomcat/commit/9ffd23fc27f5d1fc95bf97e5cea175c8968f4533 (9.0.98), https://github.com/apache/tomcat/commit/a95bf2b0303442a2c9a1ac364b0e63b56049e33a, https://github.com/apache/tomcat/commit/aa5b4d0043289cf054f531ec55126c980d3572e1, https://github.com/apache/tomcat/commit/aa5b4d0043289cf054f531ec55126c980d3572e1 (10.1.34), https://github.com/apache/tomcat/commit/bbd82e9593314ade4cfd57248f9285fbad686f66, https://github.com/apache/tomcat/commit/bbd82e9593314ade4cfd57248f9285fbad686f66 (10.1.34), https://github.com/apache/tomcat/commit/c0a23927ea5e061ca3fdff695138464179fe674a, https://github.com/apache/tomcat/commit/c2f7ce21c3fb12caefee87c517a8bb4f80700044, https://github.com/apache/tomcat/commit/c2f7ce21c3fb12caefee87c517a8bb4f80700044 (9.0.98), https://github.com/apache/tomcat/commit/cb1707685472994e9d924746f8c91cb116fa5213, https://github.com/apache/tomcat/commit/d63a10afc142b12f462a15f7d10f79fd80ff94eb, https://github.com/apache/tomcat/commit/d63a10afc142b12f462a15f7d10f79fd80ff94eb (10.1.34), https://github.com/apache/tomcat/commit/dbec927859d9484cb8bd680a7c67b1a560f48444, https://github.com/apache/tomcat/commit/dbec927859d9484cb8bd680a7c67b1a560f48444 (10.1.34), https://github.com/apache/tomcat/commit/e8c16cdba833884e1bd49fff1f1cb699da177585, https://github.com/apache/tomcat/commit/e8c16cdba833884e1bd49fff1f1cb699da177585 (10.1.34), https://github.com/apache/tomcat/commit/f57a9d9847c1038be61f5818d73b8be907c460d4, https://github.com/apache/tomcat/commit/f57a9d9847c1038be61f5818d73b8be907c460d4 (10.1.34), https://linux.oracle.com/cve/CVE-2024-54677.html, https://linux.oracle.com/errata/ELSA-2025-7497.html, https://lists.apache.org/thread/tdtbbxpg5trdwc2wnopcth9ccvdftq2n, https://nvd.nist.gov/vuln/detail/CVE-2024-54677, https://security.netapp.com/advisory/ntap-20250131-0006, https://security.netapp.com/advisory/ntap-20250131-0006/, https://tomcat.apache.org/security-10.html#Fixed_in_Apache_Tomcat_10.1.34, https://tomcat.apache.org/security-11.html#Fixed_in_Apache_Tomcat_11.0.2, https://tomcat.apache.org/security-9.html#Fixed_in_Apache_Tomcat_9.0.98, https://www.cve.org/CVERecord?id=CVE-2024-54677</t>
+          <t>http://www.openwall.com/lists/oss-security/2024/12/17/5, http://www.openwall.com/lists/oss-security/2024/12/17/6, http://www.openwall.com/lists/oss-security/2024/12/18/1, https://access.redhat.com/errata/RHSA-2025:7497, https://access.redhat.com/security/cve/CVE-2024-54677, https://bugzilla.redhat.com/2326972, https://bugzilla.redhat.com/2332815, https://bugzilla.redhat.com/2351129, https://errata.almalinux.org/10/ALSA-2025-7497.html, https://github.com/apache/tomcat, https://github.com/apache/tomcat/commit/1d88dd3ffaed76188dd4ee32ce77709ce6e153cd, https://github.com/apache/tomcat/commit/1d88dd3ffaed76188dd4ee32ce77709ce6e153cd (9.0.98), https://github.com/apache/tomcat/commit/3315a9027a7eaab18f42625b97b569940ff1365d, https://github.com/apache/tomcat/commit/3315a9027a7eaab18f42625b97b569940ff1365d (9.0.98), https://github.com/apache/tomcat/commit/4a335c6dcba8d6f8a54629eda392a50da267bdf4, https://github.com/apache/tomcat/commit/4d5cc6538d91386f950373ac8120e98c2c78ed3a, https://github.com/apache/tomcat/commit/4d5cc6538d91386f950373ac8120e98c2c78ed3a (9.0.98), https://github.com/apache/tomcat/commit/4f0236606961176257b883213e1621b1859ed746, https://github.com/apache/tomcat/commit/54e56495e9a106218efe9fc9c79d976c0032bbfd, https://github.com/apache/tomcat/commit/54e56495e9a106218efe9fc9c79d976c0032bbfd (10.1.34), https://github.com/apache/tomcat/commit/721544ea28e92549824b106be954a9f411867a1c, https://github.com/apache/tomcat/commit/721544ea28e92549824b106be954a9f411867a1c (9.0.98), https://github.com/apache/tomcat/commit/722814668708c42a61b0c1e340b15bc2b785c0d1, https://github.com/apache/tomcat/commit/75ff7e8622edcc024b268677aa789ee8f0880ecc, https://github.com/apache/tomcat/commit/75ff7e8622edcc024b268677aa789ee8f0880ecc (9.0.98), https://github.com/apache/tomcat/commit/84065e26ca4555e63a922bb29b13b0a1c86b7654, https://github.com/apache/tomcat/commit/84065e26ca4555e63a922bb29b13b0a1c86b7654 (9.0.98), https://github.com/apache/tomcat/commit/84c4af76e7a10fc7f8630ce62e6a46632ea4a90e, https://github.com/apache/tomcat/commit/84c4af76e7a10fc7f8630ce62e6a46632ea4a90e (9.0.98), https://github.com/apache/tomcat/commit/9ffd23fc27f5d1fc95bf97e5cea175c8968f4533, https://github.com/apache/tomcat/commit/9ffd23fc27f5d1fc95bf97e5cea175c8968f4533 (9.0.98), https://github.com/apache/tomcat/commit/a95bf2b0303442a2c9a1ac364b0e63b56049e33a, https://github.com/apache/tomcat/commit/aa5b4d0043289cf054f531ec55126c980d3572e1, https://github.com/apache/tomcat/commit/aa5b4d0043289cf054f531ec55126c980d3572e1 (10.1.34), https://github.com/apache/tomcat/commit/bbd82e9593314ade4cfd57248f9285fbad686f66, https://github.com/apache/tomcat/commit/bbd82e9593314ade4cfd57248f9285fbad686f66 (10.1.34), https://github.com/apache/tomcat/commit/c0a23927ea5e061ca3fdff695138464179fe674a, https://github.com/apache/tomcat/commit/c2f7ce21c3fb12caefee87c517a8bb4f80700044, https://github.com/apache/tomcat/commit/c2f7ce21c3fb12caefee87c517a8bb4f80700044 (9.0.98), https://github.com/apache/tomcat/commit/cb1707685472994e9d924746f8c91cb116fa5213, https://github.com/apache/tomcat/commit/d63a10afc142b12f462a15f7d10f79fd80ff94eb, https://github.com/apache/tomcat/commit/d63a10afc142b12f462a15f7d10f79fd80ff94eb (10.1.34), https://github.com/apache/tomcat/commit/dbec927859d9484cb8bd680a7c67b1a560f48444, https://github.com/apache/tomcat/commit/dbec927859d9484cb8bd680a7c67b1a560f48444 (10.1.34), https://github.com/apache/tomcat/commit/e8c16cdba833884e1bd49fff1f1cb699da177585, https://github.com/apache/tomcat/commit/e8c16cdba833884e1bd49fff1f1cb699da177585 (10.1.34), https://github.com/apache/tomcat/commit/f57a9d9847c1038be61f5818d73b8be907c460d4, https://github.com/apache/tomcat/commit/f57a9d9847c1038be61f5818d73b8be907c460d4 (10.1.34), https://linux.oracle.com/cve/CVE-2024-54677.html, https://linux.oracle.com/errata/ELSA-2025-7497.html, https://lists.apache.org/thread/tdtbbxpg5trdwc2wnopcth9ccvdftq2n, https://nvd.nist.gov/vuln/detail/CVE-2024-54677, https://security.netapp.com/advisory/ntap-20250131-0006, https://security.netapp.com/advisory/ntap-20250131-0006/, https://tomcat.apache.org/security-10.html#Fixed_in_Apache_Tomcat_10.1.34, https://tomcat.apache.org/security-11.html#Fixed_in_Apache_Tomcat_11.0.2, https://tomcat.apache.org/security-9.html#Fixed_in_Apache_Tomcat_9.0.98, https://www.cve.org/CVERecord?id=CVE-2024-54677</t>
         </is>
       </c>
       <c r="J223" t="inlineStr">

</xml_diff>